<commit_message>
Add conditional format tests
</commit_message>
<xml_diff>
--- a/tests/Templates/ConditionalFormat.xlsx
+++ b/tests/Templates/ConditionalFormat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\_CodeOS\ClosedXML.Report\tests\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E1F28A-7E40-4505-921F-C04179D3BB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45060B44-39D3-4699-A667-563C6C505F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="1350" windowWidth="30120" windowHeight="15780" xr2:uid="{08B6BED3-118D-4C3F-889E-3A36F49C849F}"/>
+    <workbookView xWindow="1020" yWindow="1470" windowWidth="30120" windowHeight="15780" xr2:uid="{08B6BED3-118D-4C3F-889E-3A36F49C849F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,19 +91,19 @@
     <t>&lt;&lt;ConditionalFormat json={
     "rules": [
         {
-            "ruleType": "between",
-            "from": 0,
-            "to": 1000,
+            "operator": "between",
+            "minValue": 0,
+            "maxValue": 1000,
             "background": "#E2FEE2"
         },
         {
-            "ruleType": "between",
-            "from": 1001,
-            "to": 10000,
+            "operator": "between",
+            "minValue": 1001,
+            "maxValue": 10000,
             "background": "#FFFFD4"
         },
         {
-            "ruleType": "greaterThan",
+            "operator": "greaterThan",
             "value": 100001,
             "background": "#FB8383"
         }
@@ -529,7 +529,7 @@
   <dimension ref="B2:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>